<commit_message>
changed holdEnterDate from LocalDate to LocalDateTime
</commit_message>
<xml_diff>
--- a/acm-standard-applications/acm-foia/src/main/resources/rules/drools-case-file-rules-foia.xlsx
+++ b/acm-standard-applications/acm-foia/src/main/resources/rules/drools-case-file-rules-foia.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ana.serafimoska\IdeaProjects\ArkCase\acm-standard-applications\acm-foia\src\main\resources\rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ArkcaseProjects\ArkCase\acm-standard-applications\acm-foia\src\main\resources\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35503545-F82F-45E4-9B0B-057D2F539BB1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEE2144F-D265-451B-998F-710D5FFCF1E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="8190" tabRatio="111" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="111" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -179,9 +179,6 @@
     <t>setBillingEnterDate, null</t>
   </si>
   <si>
-    <t>setHoldEnterDate, java.time.LocalDate.now()</t>
-  </si>
-  <si>
     <t>Set Hold Enter Date</t>
   </si>
   <si>
@@ -285,6 +282,9 @@
   </si>
   <si>
     <t>setQueueEnterDate, java.time.LocalDateTime.now()</t>
+  </si>
+  <si>
+    <t>setHoldEnterDate, java.time.LocalDateTime.now()</t>
   </si>
 </sst>
 </file>
@@ -1005,20 +1005,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="C19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.42578125"/>
-    <col min="2" max="2" width="47.5703125" customWidth="1"/>
+    <col min="1" max="1" width="19.453125"/>
+    <col min="2" max="2" width="47.54296875" customWidth="1"/>
     <col min="3" max="3" width="130" customWidth="1"/>
-    <col min="4" max="4" width="100.42578125"/>
-    <col min="5" max="5" width="27.7109375"/>
+    <col min="4" max="4" width="100.453125"/>
+    <col min="5" max="5" width="27.7265625"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="2" t="s">
@@ -1028,17 +1028,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="21" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="4" t="s">
@@ -1048,7 +1048,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="4" t="s">
@@ -1058,7 +1058,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="4" t="s">
@@ -1068,7 +1068,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="4" t="s">
@@ -1078,7 +1078,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="4" t="s">
@@ -1088,7 +1088,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="4" t="s">
@@ -1098,7 +1098,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="4" t="s">
@@ -1108,7 +1108,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="4" t="s">
@@ -1118,7 +1118,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="4" t="s">
@@ -1128,7 +1128,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="4" t="s">
@@ -1138,7 +1138,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="4" t="s">
@@ -1148,7 +1148,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="330" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="319" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="4" t="s">
@@ -1158,7 +1158,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="8" t="s">
@@ -1168,7 +1168,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="2" t="s">
@@ -1176,7 +1176,7 @@
       </c>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="4" t="s">
@@ -1186,7 +1186,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="4" t="s">
@@ -1194,7 +1194,7 @@
       </c>
       <c r="D20" s="10"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="11" t="s">
@@ -1204,7 +1204,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A22" s="13" t="s">
         <v>21</v>
       </c>
@@ -1218,7 +1218,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
       <c r="B23" s="17" t="s">
         <v>25</v>
@@ -1230,7 +1230,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
       <c r="B24" s="17" t="s">
         <v>28</v>
@@ -1242,7 +1242,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="B25" s="17" t="s">
         <v>31</v>
@@ -1254,7 +1254,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
       <c r="B26" s="17" t="s">
         <v>34</v>
@@ -1266,197 +1266,197 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
       <c r="B27" s="17" t="s">
         <v>37</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D27" s="17" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="1"/>
       <c r="B28" s="17" t="s">
         <v>38</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="1"/>
       <c r="B29" s="17" t="s">
         <v>42</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D29" s="17" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="1"/>
       <c r="B30" s="17" t="s">
         <v>44</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D30" s="17" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="1"/>
       <c r="B31" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="1"/>
       <c r="B32" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C32" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="D32" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="C32" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="D32" s="17" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="1"/>
       <c r="B33" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="C33" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="C33" s="17" t="s">
-        <v>58</v>
-      </c>
       <c r="D33" s="17" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="1"/>
       <c r="B34" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C34" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="C34" s="17" t="s">
-        <v>60</v>
-      </c>
       <c r="D34" s="17" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="1"/>
       <c r="B35" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C35" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="C35" s="17" t="s">
-        <v>72</v>
-      </c>
       <c r="D35" s="17" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="1"/>
       <c r="B36" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="C36" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="C36" s="17" t="s">
-        <v>62</v>
-      </c>
       <c r="D36" s="17" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="1"/>
       <c r="B37" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C37" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="C37" s="17" t="s">
-        <v>64</v>
-      </c>
       <c r="D37" s="17" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="1"/>
       <c r="B38" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C38" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="C38" s="17" t="s">
-        <v>66</v>
-      </c>
       <c r="D38" s="17" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="1"/>
       <c r="B39" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C39" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="C39" s="17" t="s">
-        <v>68</v>
-      </c>
       <c r="D39" s="17" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="1"/>
       <c r="B40" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C40" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="C40" s="17" t="s">
-        <v>56</v>
-      </c>
       <c r="D40" s="17" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="1"/>
       <c r="B41" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="C41" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="D41" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="C41" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="D41" s="19" t="s">
-        <v>70</v>
-      </c>
       <c r="E41" s="20"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="1"/>
       <c r="B42" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="C42" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="D42" s="19" t="s">
         <v>74</v>
-      </c>
-      <c r="C42" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="D42" s="19" t="s">
-        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1471,7 +1471,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -1484,7 +1484,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
ACFP-1185 FOIA: Request are not shown in the Hold queue table, when queue is changed in Hold
</commit_message>
<xml_diff>
--- a/acm-standard-applications/acm-foia/src/main/resources/rules/drools-case-file-rules-foia.xlsx
+++ b/acm-standard-applications/acm-foia/src/main/resources/rules/drools-case-file-rules-foia.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ArkcaseProjects\ArkCase\acm-standard-applications\acm-foia\src\main\resources\rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ana.serafimoska\IdeaProjects\ArkCase\acm-standard-applications\acm-foia\src\main\resources\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEE2144F-D265-451B-998F-710D5FFCF1E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{220A3BCB-7DC2-4B73-A703-A49D24DC6CBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="111" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="111" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -170,9 +170,6 @@
     <t>Set Biiling Enter Date</t>
   </si>
   <si>
-    <t>setBillingEnterDate, java.time.LocalDate.now()</t>
-  </si>
-  <si>
     <t>Nullify Billing Enter Date</t>
   </si>
   <si>
@@ -285,6 +282,9 @@
   </si>
   <si>
     <t>setHoldEnterDate, java.time.LocalDateTime.now()</t>
+  </si>
+  <si>
+    <t>setBillingEnterDate, java.time.LocalDateTime.now()</t>
   </si>
 </sst>
 </file>
@@ -1006,19 +1006,19 @@
   <dimension ref="A2:E42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.453125"/>
-    <col min="2" max="2" width="47.54296875" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125"/>
+    <col min="2" max="2" width="47.5703125" customWidth="1"/>
     <col min="3" max="3" width="130" customWidth="1"/>
-    <col min="4" max="4" width="100.453125"/>
-    <col min="5" max="5" width="27.7265625"/>
+    <col min="4" max="4" width="100.42578125"/>
+    <col min="5" max="5" width="27.7109375"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="2" t="s">
@@ -1028,17 +1028,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="21" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="4" t="s">
@@ -1048,7 +1048,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="4" t="s">
@@ -1058,7 +1058,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="4" t="s">
@@ -1068,7 +1068,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="4" t="s">
@@ -1078,7 +1078,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="4" t="s">
@@ -1088,7 +1088,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="4" t="s">
@@ -1098,7 +1098,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="4" t="s">
@@ -1108,7 +1108,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="4" t="s">
@@ -1118,7 +1118,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="4" t="s">
@@ -1128,7 +1128,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="4" t="s">
@@ -1138,7 +1138,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="4" t="s">
@@ -1148,7 +1148,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="319" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" ht="330" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="4" t="s">
@@ -1158,7 +1158,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="8" t="s">
@@ -1168,7 +1168,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="2" t="s">
@@ -1176,7 +1176,7 @@
       </c>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="4" t="s">
@@ -1186,7 +1186,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="4" t="s">
@@ -1194,7 +1194,7 @@
       </c>
       <c r="D20" s="10"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="11" t="s">
@@ -1204,7 +1204,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
         <v>21</v>
       </c>
@@ -1218,7 +1218,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="17" t="s">
         <v>25</v>
@@ -1230,7 +1230,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="17" t="s">
         <v>28</v>
@@ -1242,7 +1242,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="17" t="s">
         <v>31</v>
@@ -1254,7 +1254,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="17" t="s">
         <v>34</v>
@@ -1266,197 +1266,197 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="17" t="s">
         <v>37</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D27" s="17" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="17" t="s">
         <v>38</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="17" t="s">
         <v>42</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D29" s="17" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D30" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="C30" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="D30" s="17" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C32" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="D32" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="C32" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="D32" s="17" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C33" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="C33" s="17" t="s">
-        <v>57</v>
-      </c>
       <c r="D33" s="17" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="C34" s="17" t="s">
-        <v>59</v>
-      </c>
       <c r="D34" s="17" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="C35" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="C35" s="17" t="s">
-        <v>71</v>
-      </c>
       <c r="D35" s="17" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="C36" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C36" s="17" t="s">
-        <v>61</v>
-      </c>
       <c r="D36" s="17" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C37" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="C37" s="17" t="s">
-        <v>63</v>
-      </c>
       <c r="D37" s="17" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C38" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="C38" s="17" t="s">
-        <v>65</v>
-      </c>
       <c r="D38" s="17" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="C39" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="C39" s="17" t="s">
-        <v>67</v>
-      </c>
       <c r="D39" s="17" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C40" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="C40" s="17" t="s">
-        <v>55</v>
-      </c>
       <c r="D40" s="17" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C41" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="D41" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="C41" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="D41" s="19" t="s">
-        <v>69</v>
-      </c>
       <c r="E41" s="20"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="C42" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="D42" s="19" t="s">
         <v>73</v>
-      </c>
-      <c r="C42" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="D42" s="19" t="s">
-        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1471,7 +1471,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -1484,7 +1484,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>